<commit_message>
Abordagem - removal_ha (sem -)
</commit_message>
<xml_diff>
--- a/output/est-removals-ha-biome.xlsx
+++ b/output/est-removals-ha-biome.xlsx
@@ -394,13 +394,13 @@
         </is>
       </c>
       <c r="C2">
-        <v>-323906754.379146</v>
+        <v>50332051.47490814</v>
       </c>
       <c r="D2">
-        <v>2091798884.266725</v>
+        <v>773500144.8783754</v>
       </c>
       <c r="E2">
-        <v>-154.8460307610742</v>
+        <v>65.07051331299016</v>
       </c>
     </row>
     <row r="3">
@@ -413,13 +413,13 @@
         </is>
       </c>
       <c r="C3">
-        <v>685982766.5406247</v>
+        <v>781794475.4946911</v>
       </c>
       <c r="D3">
-        <v>5616477035.427435</v>
+        <v>4863993091.163775</v>
       </c>
       <c r="E3">
-        <v>122.1375538818381</v>
+        <v>160.7310004027239</v>
       </c>
     </row>
     <row r="4">
@@ -432,13 +432,13 @@
         </is>
       </c>
       <c r="C4">
-        <v>-272603694.4970437</v>
+        <v>12417625.785737</v>
       </c>
       <c r="D4">
-        <v>1429327349.611023</v>
+        <v>202668507.2253587</v>
       </c>
       <c r="E4">
-        <v>-190.7216667834909</v>
+        <v>61.27062342216361</v>
       </c>
     </row>
     <row r="5">
@@ -451,13 +451,13 @@
         </is>
       </c>
       <c r="C5">
-        <v>133325351.556758</v>
+        <v>240879170.3501668</v>
       </c>
       <c r="D5">
-        <v>2500212128.95899</v>
+        <v>1667710662.935601</v>
       </c>
       <c r="E5">
-        <v>53.32561585975127</v>
+        <v>144.4370271796172</v>
       </c>
     </row>
     <row r="6">
@@ -470,13 +470,13 @@
         </is>
       </c>
       <c r="C6">
-        <v>29730567.8439153</v>
+        <v>32271138.3268733</v>
       </c>
       <c r="D6">
-        <v>227125558.0243705</v>
+        <v>168243183.6822288</v>
       </c>
       <c r="E6">
-        <v>130.8992616353868</v>
+        <v>191.8124563538085</v>
       </c>
     </row>
     <row r="7">
@@ -508,13 +508,13 @@
         </is>
       </c>
       <c r="C8">
-        <v>485398301.4161426</v>
+        <v>501203201.3946835</v>
       </c>
       <c r="D8">
-        <v>2091798884.266725</v>
+        <v>1573907746.592665</v>
       </c>
       <c r="E8">
-        <v>232.0482648054848</v>
+        <v>318.4450946885119</v>
       </c>
     </row>
     <row r="9">
@@ -527,13 +527,13 @@
         </is>
       </c>
       <c r="C9">
-        <v>1660479082.564546</v>
+        <v>1715879494.422725</v>
       </c>
       <c r="D9">
-        <v>5616477035.427435</v>
+        <v>4929796264.592522</v>
       </c>
       <c r="E9">
-        <v>295.6442396346728</v>
+        <v>348.0629629152745</v>
       </c>
     </row>
     <row r="10">
@@ -546,13 +546,13 @@
         </is>
       </c>
       <c r="C10">
-        <v>514840189.9226552</v>
+        <v>516414783.6085377</v>
       </c>
       <c r="D10">
-        <v>1429327349.611023</v>
+        <v>1413441928.104768</v>
       </c>
       <c r="E10">
-        <v>360.1975363185792</v>
+        <v>365.3597458375804</v>
       </c>
     </row>
     <row r="11">
@@ -565,13 +565,13 @@
         </is>
       </c>
       <c r="C11">
-        <v>878391192.6120528</v>
+        <v>894385832.9471077</v>
       </c>
       <c r="D11">
-        <v>2500212128.95899</v>
+        <v>2315684868.422894</v>
       </c>
       <c r="E11">
-        <v>351.3266664208158</v>
+        <v>386.2295103893962</v>
       </c>
     </row>
     <row r="12">
@@ -584,13 +584,13 @@
         </is>
       </c>
       <c r="C12">
-        <v>38580707.34233644</v>
+        <v>43612244.87203784</v>
       </c>
       <c r="D12">
-        <v>227125558.0243705</v>
+        <v>179011937.08526</v>
       </c>
       <c r="E12">
-        <v>169.8651075551644</v>
+        <v>243.6275791556076</v>
       </c>
     </row>
     <row r="13">
@@ -603,13 +603,13 @@
         </is>
       </c>
       <c r="C13">
-        <v>80785798.2465</v>
+        <v>80814206.242</v>
       </c>
       <c r="D13">
-        <v>214433403.7632375</v>
+        <v>214025158.8077344</v>
       </c>
       <c r="E13">
-        <v>376.7407354858672</v>
+        <v>377.5920863331679</v>
       </c>
     </row>
     <row r="14">
@@ -622,13 +622,13 @@
         </is>
       </c>
       <c r="C14">
-        <v>41282749.8188653</v>
+        <v>89621261.04626356</v>
       </c>
       <c r="D14">
-        <v>2091798884.266725</v>
+        <v>1500091513.779432</v>
       </c>
       <c r="E14">
-        <v>19.73552530760474</v>
+        <v>59.74386243974256</v>
       </c>
     </row>
     <row r="15">
@@ -641,13 +641,13 @@
         </is>
       </c>
       <c r="C15">
-        <v>1063160075.171129</v>
+        <v>1078061040.322272</v>
       </c>
       <c r="D15">
-        <v>5616477035.427435</v>
+        <v>5146429395.837155</v>
       </c>
       <c r="E15">
-        <v>189.293051224987</v>
+        <v>209.477476013621</v>
       </c>
     </row>
     <row r="16">
@@ -660,13 +660,13 @@
         </is>
       </c>
       <c r="C16">
-        <v>29530305.1327424</v>
+        <v>70465079.67538077</v>
       </c>
       <c r="D16">
-        <v>1429327349.611023</v>
+        <v>794201029.9429028</v>
       </c>
       <c r="E16">
-        <v>20.66028131398925</v>
+        <v>88.7244879050921</v>
       </c>
     </row>
     <row r="17">
@@ -679,13 +679,13 @@
         </is>
       </c>
       <c r="C17">
-        <v>481811277.8890184</v>
+        <v>485991296.3443565</v>
       </c>
       <c r="D17">
-        <v>2500212128.95899</v>
+        <v>2437592220.690554</v>
       </c>
       <c r="E17">
-        <v>192.7081595630965</v>
+        <v>199.3735015312275</v>
       </c>
     </row>
     <row r="18">
@@ -698,13 +698,13 @@
         </is>
       </c>
       <c r="C18">
-        <v>-13519842.35150353</v>
+        <v>4964423.86935757</v>
       </c>
       <c r="D18">
-        <v>227125558.0243705</v>
+        <v>77631574.8399705</v>
       </c>
       <c r="E18">
-        <v>-59.52585199615823</v>
+        <v>63.94851424296388</v>
       </c>
     </row>
     <row r="19">
@@ -717,13 +717,13 @@
         </is>
       </c>
       <c r="C19">
-        <v>56891085.3447</v>
+        <v>57668708.8547</v>
       </c>
       <c r="D19">
-        <v>214433403.7632375</v>
+        <v>194082613.4405517</v>
       </c>
       <c r="E19">
-        <v>265.3088760719165</v>
+        <v>297.1348532070554</v>
       </c>
     </row>
   </sheetData>

</xml_diff>